<commit_message>
Make current working diction persist between sessions
</commit_message>
<xml_diff>
--- a/Iteration Burndown.xlsx
+++ b/Iteration Burndown.xlsx
@@ -274,13 +274,13 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1623,7 +1623,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,7 +1656,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <f>B2-(B2/14)*A3</f>
@@ -1668,7 +1668,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <f>B2-(B2/14)*A4</f>
@@ -1680,7 +1680,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <f>B2-(B2/14)*A5</f>

</xml_diff>

<commit_message>
Able to open dictions
</commit_message>
<xml_diff>
--- a/Iteration Burndown.xlsx
+++ b/Iteration Burndown.xlsx
@@ -271,46 +271,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -419,46 +419,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.071428571428571</c:v>
+                  <c:v>10.214285714285714</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.142857142857142</c:v>
+                  <c:v>9.4285714285714288</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.214285714285715</c:v>
+                  <c:v>8.6428571428571423</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2857142857142847</c:v>
+                  <c:v>7.8571428571428577</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.3571428571428577</c:v>
+                  <c:v>7.0714285714285712</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.4285714285714288</c:v>
+                  <c:v>6.2857142857142856</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6.5</c:v>
+                  <c:v>5.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.5714285714285712</c:v>
+                  <c:v>4.7142857142857144</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.6428571428571423</c:v>
+                  <c:v>3.9285714285714288</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.7142857142857135</c:v>
+                  <c:v>3.1428571428571432</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.7857142857142847</c:v>
+                  <c:v>2.3571428571428577</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.8571428571428577</c:v>
+                  <c:v>1.5714285714285712</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.92857142857142883</c:v>
+                  <c:v>0.78571428571428648</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -478,11 +478,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="324362040"/>
-        <c:axId val="324364392"/>
+        <c:axId val="314952648"/>
+        <c:axId val="314953040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="324362040"/>
+        <c:axId val="314952648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,7 +581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324364392"/>
+        <c:crossAx val="314953040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -589,7 +589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="324364392"/>
+        <c:axId val="314953040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,7 +701,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="324362040"/>
+        <c:crossAx val="314952648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1623,7 +1623,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,11 +1644,11 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <f>B2-(B2/14)*A2</f>
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1656,11 +1656,11 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <f>B2-(B2/14)*A3</f>
-        <v>12.071428571428571</v>
+        <v>10.214285714285714</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1668,11 +1668,11 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f>B2-(B2/14)*A4</f>
-        <v>11.142857142857142</v>
+        <v>9.4285714285714288</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1680,11 +1680,11 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <f>B2-(B2/14)*A5</f>
-        <v>10.214285714285715</v>
+        <v>8.6428571428571423</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1692,11 +1692,11 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C6">
         <f>B2-(B2/14)*A6</f>
-        <v>9.2857142857142847</v>
+        <v>7.8571428571428577</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1704,11 +1704,11 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C7">
         <f>B2-(B2/14)*A7</f>
-        <v>8.3571428571428577</v>
+        <v>7.0714285714285712</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1716,11 +1716,11 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <f>B2-(B2/14)*A8</f>
-        <v>7.4285714285714288</v>
+        <v>6.2857142857142856</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1728,11 +1728,11 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C9">
         <f>B2-(B2/14)*A9</f>
-        <v>6.5</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1740,11 +1740,11 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C10">
         <f>B2-(B2/14)*A10</f>
-        <v>5.5714285714285712</v>
+        <v>4.7142857142857144</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1752,11 +1752,11 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C11">
         <f>B2-(B2/14)*A11</f>
-        <v>4.6428571428571423</v>
+        <v>3.9285714285714288</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1764,11 +1764,11 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C12">
         <f>B2-(B2/14)*A12</f>
-        <v>3.7142857142857135</v>
+        <v>3.1428571428571432</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1776,11 +1776,11 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C13">
         <f>B2-(B2/14)*A13</f>
-        <v>2.7857142857142847</v>
+        <v>2.3571428571428577</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1788,11 +1788,11 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C14">
         <f>B2-(B2/14)*A14</f>
-        <v>1.8571428571428577</v>
+        <v>1.5714285714285712</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1800,11 +1800,11 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C15">
         <f>B2-(B2/14)*A15</f>
-        <v>0.92857142857142883</v>
+        <v>0.78571428571428648</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Partially implemented the comments feature
</commit_message>
<xml_diff>
--- a/Iteration Burndown.xlsx
+++ b/Iteration Burndown.xlsx
@@ -274,46 +274,46 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -478,11 +478,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="314952648"/>
-        <c:axId val="314953040"/>
+        <c:axId val="311038072"/>
+        <c:axId val="311040816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="314952648"/>
+        <c:axId val="311038072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,7 +581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314953040"/>
+        <c:crossAx val="311040816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -589,7 +589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="314953040"/>
+        <c:axId val="311040816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,7 +701,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314952648"/>
+        <c:crossAx val="311038072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1623,7 +1623,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,7 +1656,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <f>B2-(B2/14)*A3</f>
@@ -1668,7 +1668,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <f>B2-(B2/14)*A4</f>
@@ -1680,7 +1680,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <f>B2-(B2/14)*A5</f>
@@ -1692,7 +1692,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <f>B2-(B2/14)*A6</f>
@@ -1704,7 +1704,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <f>B2-(B2/14)*A7</f>
@@ -1716,7 +1716,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <f>B2-(B2/14)*A8</f>
@@ -1728,7 +1728,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C9">
         <f>B2-(B2/14)*A9</f>
@@ -1740,7 +1740,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C10">
         <f>B2-(B2/14)*A10</f>
@@ -1752,7 +1752,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <f>B2-(B2/14)*A11</f>
@@ -1764,7 +1764,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C12">
         <f>B2-(B2/14)*A12</f>
@@ -1776,7 +1776,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <f>B2-(B2/14)*A13</f>
@@ -1788,7 +1788,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C14">
         <f>B2-(B2/14)*A14</f>
@@ -1800,7 +1800,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <f>B2-(B2/14)*A15</f>
@@ -1812,7 +1812,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <f>B2-(B2/14)*A16</f>

</xml_diff>

<commit_message>
Implemented basic comment system and unit tests for Diction
</commit_message>
<xml_diff>
--- a/Iteration Burndown.xlsx
+++ b/Iteration Burndown.xlsx
@@ -131,7 +131,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Iteration 3 Burndown</a:t>
+              <a:t>Iteration 5 Burndown</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -277,43 +277,43 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -478,11 +478,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="311038072"/>
-        <c:axId val="311040816"/>
+        <c:axId val="314335496"/>
+        <c:axId val="314336280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="311038072"/>
+        <c:axId val="314335496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,7 +581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311040816"/>
+        <c:crossAx val="314336280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -589,7 +589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="311040816"/>
+        <c:axId val="314336280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,7 +701,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="311038072"/>
+        <c:crossAx val="314335496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1623,7 +1623,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1668,7 +1668,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4">
         <f>B2-(B2/14)*A4</f>
@@ -1680,7 +1680,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <f>B2-(B2/14)*A5</f>
@@ -1692,7 +1692,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6">
         <f>B2-(B2/14)*A6</f>
@@ -1704,7 +1704,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <f>B2-(B2/14)*A7</f>
@@ -1716,7 +1716,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <f>B2-(B2/14)*A8</f>
@@ -1728,7 +1728,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <f>B2-(B2/14)*A9</f>
@@ -1740,7 +1740,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10">
         <f>B2-(B2/14)*A10</f>
@@ -1764,7 +1764,7 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <f>B2-(B2/14)*A12</f>
@@ -1776,7 +1776,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <f>B2-(B2/14)*A13</f>
@@ -1788,7 +1788,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C14">
         <f>B2-(B2/14)*A14</f>
@@ -1800,7 +1800,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <f>B2-(B2/14)*A15</f>
@@ -1812,7 +1812,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C16">
         <f>B2-(B2/14)*A16</f>

</xml_diff>

<commit_message>
Iteration Report and README updated
</commit_message>
<xml_diff>
--- a/Iteration Burndown.xlsx
+++ b/Iteration Burndown.xlsx
@@ -131,7 +131,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Iteration 5 Burndown</a:t>
+              <a:t>Iteration 6 Burndown</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -271,34 +271,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>5</c:v>
@@ -307,10 +307,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -419,46 +419,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.214285714285714</c:v>
+                  <c:v>11.142857142857142</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>10.285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>9.4285714285714288</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.6428571428571423</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.8571428571428577</c:v>
+                  <c:v>8.5714285714285712</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0714285714285712</c:v>
+                  <c:v>7.7142857142857144</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.2857142857142856</c:v>
+                  <c:v>6.8571428571428577</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.7142857142857144</c:v>
+                  <c:v>5.1428571428571432</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.9285714285714288</c:v>
+                  <c:v>4.2857142857142865</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.1428571428571432</c:v>
+                  <c:v>3.4285714285714288</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.3571428571428577</c:v>
+                  <c:v>2.5714285714285712</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.5714285714285712</c:v>
+                  <c:v>1.7142857142857153</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.78571428571428648</c:v>
+                  <c:v>0.85714285714285765</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -478,11 +478,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="314335496"/>
-        <c:axId val="314336280"/>
+        <c:axId val="301128976"/>
+        <c:axId val="301130152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="314335496"/>
+        <c:axId val="301128976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -581,7 +581,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314336280"/>
+        <c:crossAx val="301130152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -589,7 +589,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="314336280"/>
+        <c:axId val="301130152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -701,7 +701,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="314335496"/>
+        <c:crossAx val="301128976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1623,7 +1623,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1644,11 +1644,11 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C2">
         <f>B2-(B2/14)*A2</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1656,11 +1656,11 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <f>B2-(B2/14)*A3</f>
-        <v>10.214285714285714</v>
+        <v>11.142857142857142</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1668,11 +1668,11 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <f>B2-(B2/14)*A4</f>
-        <v>9.4285714285714288</v>
+        <v>10.285714285714286</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1680,11 +1680,11 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <f>B2-(B2/14)*A5</f>
-        <v>8.6428571428571423</v>
+        <v>9.4285714285714288</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1692,11 +1692,11 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6">
         <f>B2-(B2/14)*A6</f>
-        <v>7.8571428571428577</v>
+        <v>8.5714285714285712</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1704,11 +1704,11 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <f>B2-(B2/14)*A7</f>
-        <v>7.0714285714285712</v>
+        <v>7.7142857142857144</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1716,11 +1716,11 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <f>B2-(B2/14)*A8</f>
-        <v>6.2857142857142856</v>
+        <v>6.8571428571428577</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="C9">
         <f>B2-(B2/14)*A9</f>
-        <v>5.5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1740,11 +1740,11 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <f>B2-(B2/14)*A10</f>
-        <v>4.7142857142857144</v>
+        <v>5.1428571428571432</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1752,11 +1752,11 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <f>B2-(B2/14)*A11</f>
-        <v>3.9285714285714288</v>
+        <v>4.2857142857142865</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1768,7 +1768,7 @@
       </c>
       <c r="C12">
         <f>B2-(B2/14)*A12</f>
-        <v>3.1428571428571432</v>
+        <v>3.4285714285714288</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1780,7 +1780,7 @@
       </c>
       <c r="C13">
         <f>B2-(B2/14)*A13</f>
-        <v>2.3571428571428577</v>
+        <v>2.5714285714285712</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1788,11 +1788,11 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C14">
         <f>B2-(B2/14)*A14</f>
-        <v>1.5714285714285712</v>
+        <v>1.7142857142857153</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1800,11 +1800,11 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <f>B2-(B2/14)*A15</f>
-        <v>0.78571428571428648</v>
+        <v>0.85714285714285765</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>